<commit_message>
backup before adding nearcognates to physiologically representative ensembles figures
</commit_message>
<xml_diff>
--- a/src/codonValues.xlsx
+++ b/src/codonValues.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akshay/Documents/TranslationDynamics/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8206F4FA-5571-A24B-82B6-E62A88192642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D60F698-2207-DA41-966F-B50530E13E05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="1680" windowWidth="26840" windowHeight="15940" xr2:uid="{382C8ACD-C0AF-2440-A813-B863F0D59BAF}"/>
+    <workbookView xWindow="10080" yWindow="460" windowWidth="26840" windowHeight="15940" xr2:uid="{382C8ACD-C0AF-2440-A813-B863F0D59BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>GGA</t>
   </si>
@@ -574,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19395223-B780-624B-8674-63EDE490B973}">
-  <dimension ref="A1:N63"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F63" sqref="A63:F63"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1830,25 +1831,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
-        <v>2.95</v>
-      </c>
-      <c r="B63" s="2">
-        <v>3.16</v>
-      </c>
-      <c r="C63" s="2">
-        <v>3.48</v>
-      </c>
-      <c r="D63" s="2">
-        <v>3.69</v>
-      </c>
-      <c r="E63" s="2">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>23</v>
-      </c>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>